<commit_message>
Added project report and ppt
</commit_message>
<xml_diff>
--- a/data/sd_crimes.xlsx
+++ b/data/sd_crimes.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26519"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="16020" yWindow="0" windowWidth="25640" windowHeight="17540" tabRatio="500"/>
+    <workbookView xWindow="15000" yWindow="900" windowWidth="25640" windowHeight="17540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1286,10 +1286,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T47"/>
+  <dimension ref="A1:U47"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="P1" workbookViewId="0">
-      <selection activeCell="T33" sqref="T33"/>
+      <selection activeCell="V29" sqref="V29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1309,7 +1309,7 @@
     <col min="14" max="14" width="7.83203125" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20">
+    <row r="1" spans="1:21">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1353,7 +1353,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:20">
+    <row r="2" spans="1:21">
       <c r="A2" t="s">
         <v>26</v>
       </c>
@@ -1373,7 +1373,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:20">
+    <row r="3" spans="1:21">
       <c r="A3" t="s">
         <v>27</v>
       </c>
@@ -1417,7 +1417,7 @@
         <v>4.8</v>
       </c>
     </row>
-    <row r="4" spans="1:20">
+    <row r="4" spans="1:21">
       <c r="A4" t="s">
         <v>28</v>
       </c>
@@ -1461,7 +1461,7 @@
         <v>5.8</v>
       </c>
     </row>
-    <row r="5" spans="1:20">
+    <row r="5" spans="1:21">
       <c r="A5" t="s">
         <v>31</v>
       </c>
@@ -1505,7 +1505,7 @@
         <v>7.3</v>
       </c>
     </row>
-    <row r="6" spans="1:20">
+    <row r="6" spans="1:21">
       <c r="A6" t="s">
         <v>29</v>
       </c>
@@ -1519,7 +1519,7 @@
       <c r="M6" s="6"/>
       <c r="N6" s="5"/>
     </row>
-    <row r="7" spans="1:20">
+    <row r="7" spans="1:21">
       <c r="A7" t="s">
         <v>30</v>
       </c>
@@ -1537,7 +1537,7 @@
         <v>5.7</v>
       </c>
     </row>
-    <row r="8" spans="1:20">
+    <row r="8" spans="1:21">
       <c r="A8" t="s">
         <v>32</v>
       </c>
@@ -1554,7 +1554,7 @@
         <v>4.7</v>
       </c>
     </row>
-    <row r="9" spans="1:20">
+    <row r="9" spans="1:21">
       <c r="A9" t="s">
         <v>33</v>
       </c>
@@ -1596,7 +1596,7 @@
         <v>8.1999999999999993</v>
       </c>
     </row>
-    <row r="10" spans="1:20">
+    <row r="10" spans="1:21">
       <c r="A10" t="s">
         <v>18</v>
       </c>
@@ -1640,7 +1640,7 @@
         <v>6.9</v>
       </c>
     </row>
-    <row r="11" spans="1:20">
+    <row r="11" spans="1:21">
       <c r="A11" t="s">
         <v>22</v>
       </c>
@@ -1679,7 +1679,7 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="12" spans="1:20">
+    <row r="12" spans="1:21">
       <c r="A12" t="s">
         <v>34</v>
       </c>
@@ -1699,7 +1699,7 @@
         <v>3.6</v>
       </c>
     </row>
-    <row r="13" spans="1:20">
+    <row r="13" spans="1:21">
       <c r="A13" t="s">
         <v>25</v>
       </c>
@@ -1715,11 +1715,8 @@
       <c r="N13" s="3">
         <v>5.8</v>
       </c>
-      <c r="R13">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="14" spans="1:20">
+    </row>
+    <row r="14" spans="1:21">
       <c r="A14" t="s">
         <v>35</v>
       </c>
@@ -1735,14 +1732,17 @@
       <c r="N14" s="3">
         <v>8.4</v>
       </c>
-      <c r="R14">
-        <v>215</v>
+      <c r="S14">
+        <v>20</v>
       </c>
       <c r="T14">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="15" spans="1:20">
+        <v>47</v>
+      </c>
+      <c r="U14">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21">
       <c r="A15" t="s">
         <v>36</v>
       </c>
@@ -1785,11 +1785,17 @@
       <c r="N15" s="3">
         <v>8.8000000000000007</v>
       </c>
-      <c r="R15">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="16" spans="1:20">
+      <c r="S15">
+        <v>97</v>
+      </c>
+      <c r="T15">
+        <v>304</v>
+      </c>
+      <c r="U15">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21">
       <c r="A16" t="s">
         <v>38</v>
       </c>
@@ -1799,11 +1805,17 @@
       <c r="N16" s="3">
         <v>5.3</v>
       </c>
-      <c r="R16">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="17" spans="1:20">
+      <c r="S16">
+        <v>22</v>
+      </c>
+      <c r="T16">
+        <v>33</v>
+      </c>
+      <c r="U16">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:21">
       <c r="A17" t="s">
         <v>37</v>
       </c>
@@ -1846,11 +1858,17 @@
       <c r="N17" s="3">
         <v>2.2999999999999998</v>
       </c>
-      <c r="R17">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="18" spans="1:20">
+      <c r="S17">
+        <v>13</v>
+      </c>
+      <c r="T17">
+        <v>31</v>
+      </c>
+      <c r="U17">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="18" spans="1:21">
       <c r="A18" t="s">
         <v>39</v>
       </c>
@@ -1893,11 +1911,8 @@
       <c r="N18" s="3">
         <v>6.3</v>
       </c>
-      <c r="R18">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="19" spans="1:20">
+    </row>
+    <row r="19" spans="1:21">
       <c r="A19" t="s">
         <v>40</v>
       </c>
@@ -1908,14 +1923,8 @@
       <c r="N19" s="3">
         <v>5.2</v>
       </c>
-      <c r="R19">
-        <v>19</v>
-      </c>
-      <c r="T19">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="20" spans="1:20">
+    </row>
+    <row r="20" spans="1:21">
       <c r="A20" t="s">
         <v>41</v>
       </c>
@@ -1932,11 +1941,8 @@
       <c r="N20" s="3">
         <v>6.2</v>
       </c>
-      <c r="R20">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="21" spans="1:20">
+    </row>
+    <row r="21" spans="1:21">
       <c r="A21" t="s">
         <v>42</v>
       </c>
@@ -1952,11 +1958,17 @@
       <c r="N21" s="3">
         <v>5.8</v>
       </c>
-      <c r="R21">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="22" spans="1:20">
+      <c r="S21">
+        <v>4</v>
+      </c>
+      <c r="T21">
+        <v>14</v>
+      </c>
+      <c r="U21">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:21">
       <c r="A22" t="s">
         <v>43</v>
       </c>
@@ -1999,14 +2011,8 @@
       <c r="N22" s="3">
         <v>3.9</v>
       </c>
-      <c r="R22">
-        <v>241</v>
-      </c>
-      <c r="T22">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="23" spans="1:20">
+    </row>
+    <row r="23" spans="1:21">
       <c r="A23" t="s">
         <v>44</v>
       </c>
@@ -2043,19 +2049,13 @@
       <c r="L23">
         <v>8</v>
       </c>
-      <c r="R23">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="24" spans="1:20">
+    </row>
+    <row r="24" spans="1:21">
       <c r="A24" t="s">
         <v>50</v>
       </c>
-      <c r="R24">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="25" spans="1:20">
+    </row>
+    <row r="25" spans="1:21">
       <c r="A25" t="s">
         <v>51</v>
       </c>
@@ -2090,7 +2090,7 @@
         <v>5.4</v>
       </c>
     </row>
-    <row r="26" spans="1:20">
+    <row r="26" spans="1:21">
       <c r="A26" t="s">
         <v>52</v>
       </c>
@@ -2131,17 +2131,17 @@
         <v>7.3</v>
       </c>
     </row>
-    <row r="27" spans="1:20">
+    <row r="27" spans="1:21">
       <c r="A27" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="28" spans="1:20">
+    <row r="28" spans="1:21">
       <c r="A28" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="29" spans="1:20">
+    <row r="29" spans="1:21">
       <c r="A29" t="s">
         <v>55</v>
       </c>
@@ -2182,7 +2182,7 @@
         <v>8.5</v>
       </c>
     </row>
-    <row r="30" spans="1:20">
+    <row r="30" spans="1:21">
       <c r="A30" t="s">
         <v>56</v>
       </c>
@@ -2223,7 +2223,7 @@
         <v>8.6999999999999993</v>
       </c>
     </row>
-    <row r="31" spans="1:20">
+    <row r="31" spans="1:21">
       <c r="A31" t="s">
         <v>57</v>
       </c>

</xml_diff>